<commit_message>
Multiple Upload Location Changes
</commit_message>
<xml_diff>
--- a/src/assets/files/Location_Multiple sample.xlsx
+++ b/src/assets/files/Location_Multiple sample.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Location Code</t>
   </si>
@@ -27,32 +27,29 @@
     <t>Location</t>
   </si>
   <si>
-    <t>L007</t>
-  </si>
-  <si>
-    <t>melur</t>
-  </si>
-  <si>
-    <t>sample1@gmail.com</t>
-  </si>
-  <si>
-    <t>L005</t>
-  </si>
-  <si>
-    <t>chennai</t>
-  </si>
-  <si>
-    <t>sample2@gmail.com</t>
-  </si>
-  <si>
     <t>Primary Head</t>
+  </si>
+  <si>
+    <t>l007</t>
+  </si>
+  <si>
+    <t>Branch Code</t>
+  </si>
+  <si>
+    <t>b003</t>
+  </si>
+  <si>
+    <t>kesavan@gmail.com</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -64,14 +61,6 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -124,7 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -141,13 +130,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,7 +505,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -524,51 +513,49 @@
     <col min="1" max="1" width="16.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.6" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>8</v>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D3" s="6"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="B8" s="5"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="E11" s="6"/>
+      <c r="E11" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>